<commit_message>
updated bom and step files
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\foure\Documents\Projects\MZ-Switchwire\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B851BF3D-A506-456B-964A-E9D388C012C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F39ECD-C814-4911-8BF8-DF91BFA29C74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12405" yWindow="3900" windowWidth="38700" windowHeight="15435" xr2:uid="{67120B50-DA24-409C-9D35-548584692329}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="51">
   <si>
     <t>Mega Zero Switchwire Mod BOM</t>
   </si>
@@ -180,6 +180,12 @@
   </si>
   <si>
     <t>The following list of parts are applicable to modded parts. Refer to Voron Switchwire's BOM list for OEM parts.</t>
+  </si>
+  <si>
+    <t>M5x40mm Socket Head</t>
+  </si>
+  <si>
+    <t>M3x30mm Socket Head</t>
   </si>
 </sst>
 </file>
@@ -247,7 +253,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -261,6 +267,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,10 +585,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:E61"/>
+  <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -677,68 +684,80 @@
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="9">
         <v>12</v>
       </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6" t="s">
+      <c r="C10" s="5"/>
+      <c r="D10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="9">
         <v>6</v>
       </c>
     </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="B11" s="9">
+        <v>4</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="E11" s="9">
+        <v>4</v>
+      </c>
+    </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="9">
+        <v>4</v>
+      </c>
+      <c r="C12" s="5"/>
+      <c r="D12" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" s="9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="B13" s="6">
+        <v>8</v>
+      </c>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="E13" s="6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="5"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="B13" s="5">
-        <v>12</v>
-      </c>
-      <c r="C13" s="5"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="B14" s="5">
-        <v>2</v>
-      </c>
-      <c r="C14" s="5"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="B15" s="5">
-        <v>4</v>
-      </c>
+      <c r="B15" s="5"/>
       <c r="C15" s="5"/>
       <c r="D15" s="5"/>
       <c r="E15" s="5"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="B16" s="5">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="5"/>
@@ -746,7 +765,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B17" s="5">
         <v>2</v>
@@ -756,393 +775,426 @@
       <c r="E17" s="5"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B18" s="5">
+        <v>4</v>
+      </c>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="B19" s="5">
+        <v>3</v>
+      </c>
+      <c r="C19" s="5"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" s="5">
+        <v>2</v>
+      </c>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B18" s="6">
+      <c r="B21" s="6">
         <v>1</v>
       </c>
-      <c r="C18" s="6"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A20" s="4" t="s">
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B20" s="5"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="4" t="s">
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="E20" s="5"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B21" s="5">
-        <v>4</v>
-      </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="E21" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A22" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B22" s="5">
-        <v>4</v>
-      </c>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="E22" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A23" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B23" s="5">
-        <v>4</v>
-      </c>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="E23" s="5">
-        <v>4</v>
-      </c>
+      <c r="E23" s="5"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B24" s="5">
         <v>4</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E24" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B25" s="5">
+        <v>4</v>
+      </c>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E25" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="5">
+        <v>4</v>
+      </c>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="E26" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="E24" s="5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
+      <c r="B27" s="5">
+        <v>4</v>
+      </c>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B25" s="6">
-        <v>2</v>
-      </c>
-      <c r="C25" s="6"/>
-      <c r="D25" s="6" t="s">
+      <c r="B28" s="6">
+        <v>2</v>
+      </c>
+      <c r="C28" s="6"/>
+      <c r="D28" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E25" s="6">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="E28" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="7" t="s">
+      <c r="B30" s="5"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="E27" s="7"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+      <c r="E30" s="7"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B28" s="5">
-        <v>4</v>
-      </c>
-      <c r="C28" s="5"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="6" t="s">
+      <c r="B31" s="5">
+        <v>4</v>
+      </c>
+      <c r="C31" s="5"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="6">
-        <v>4</v>
-      </c>
-      <c r="C29" s="6"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+      <c r="B32" s="6">
+        <v>4</v>
+      </c>
+      <c r="C32" s="6"/>
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B31" s="5"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
-      <c r="E31" s="5"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B32" s="5">
-        <v>4</v>
-      </c>
-      <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B33" s="5">
-        <v>4</v>
-      </c>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B34" s="5">
-        <v>2</v>
-      </c>
+      <c r="B34" s="5"/>
       <c r="C34" s="5"/>
       <c r="D34" s="5"/>
       <c r="E34" s="5"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A35" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B35" s="6">
-        <v>2</v>
-      </c>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
+      <c r="A35" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B35" s="5">
+        <v>4</v>
+      </c>
+      <c r="C35" s="5"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B36" s="5">
+        <v>4</v>
+      </c>
+      <c r="C36" s="5"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B37" s="5"/>
+      <c r="A37" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B37" s="5">
+        <v>2</v>
+      </c>
       <c r="C37" s="5"/>
       <c r="D37" s="5"/>
       <c r="E37" s="5"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="B38" s="5">
-        <v>2</v>
-      </c>
-      <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
-      <c r="E38" s="5"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B39" s="5">
-        <v>12</v>
-      </c>
-      <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
-      <c r="E39" s="5"/>
+      <c r="A38" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B38" s="6">
+        <v>2</v>
+      </c>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A40" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B40" s="5">
-        <v>12</v>
-      </c>
+      <c r="A40" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B40" s="5"/>
       <c r="C40" s="5"/>
       <c r="D40" s="5"/>
       <c r="E40" s="5"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B41" s="5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="5"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B42" s="6">
+      <c r="A42" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B42" s="5">
+        <v>12</v>
+      </c>
+      <c r="C42" s="5"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A43" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" s="5">
+        <v>12</v>
+      </c>
+      <c r="C43" s="5"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A44" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B44" s="5">
         <v>3</v>
       </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="6"/>
-      <c r="E42" s="6"/>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B44" s="5"/>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="5"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B45" s="5">
-        <v>1</v>
-      </c>
-      <c r="C45" s="5"/>
-      <c r="D45" s="5"/>
-      <c r="E45" s="5"/>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="B46" s="5">
-        <v>1</v>
-      </c>
-      <c r="C46" s="5"/>
-      <c r="D46" s="5"/>
-      <c r="E46" s="5"/>
+      <c r="A45" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B45" s="6">
+        <v>3</v>
+      </c>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B47" s="5">
-        <v>2</v>
-      </c>
+      <c r="A47" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B47" s="5"/>
       <c r="C47" s="5"/>
       <c r="D47" s="5"/>
       <c r="E47" s="5"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>41</v>
+        <v>20</v>
       </c>
       <c r="B48" s="5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="5"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="6" t="s">
+      <c r="A49" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="B49" s="5">
+        <v>1</v>
+      </c>
+      <c r="C49" s="5"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B50" s="5">
+        <v>2</v>
+      </c>
+      <c r="C50" s="5"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B51" s="5">
+        <v>2</v>
+      </c>
+      <c r="C51" s="5"/>
+      <c r="D51" s="5"/>
+      <c r="E51" s="5"/>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B49" s="6">
-        <v>2</v>
-      </c>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="1" t="s">
+      <c r="B52" s="6">
+        <v>2</v>
+      </c>
+      <c r="C52" s="6"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="6"/>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>12</v>
-      </c>
-      <c r="B52">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>29</v>
-      </c>
-      <c r="B53">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>24</v>
-      </c>
-      <c r="B54">
-        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="B55">
-        <v>4</v>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>29</v>
+      </c>
+      <c r="B56">
+        <v>3</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="1" t="s">
-        <v>26</v>
+      <c r="A57" t="s">
+        <v>24</v>
+      </c>
+      <c r="B57">
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B58">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>28</v>
-      </c>
-      <c r="B59">
         <v>4</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>30</v>
-      </c>
-      <c r="B60">
-        <v>4</v>
+      <c r="A60" s="1" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
+        <v>27</v>
+      </c>
+      <c r="B61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>28</v>
+      </c>
+      <c r="B62">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>30</v>
+      </c>
+      <c r="B63">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
         <v>31</v>
       </c>
-      <c r="B61">
+      <c r="B64">
         <v>2</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D27:E29"/>
+    <mergeCell ref="D30:E32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated STEP files, BOM, and added README for Klipper configuration
</commit_message>
<xml_diff>
--- a/BOM/BOM.xlsx
+++ b/BOM/BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\foure\Documents\Projects\MZ-Switchwire\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F39ECD-C814-4911-8BF8-DF91BFA29C74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB1314BA-84E5-4533-8A5A-FC9EB52D340A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12405" yWindow="3900" windowWidth="38700" windowHeight="15435" xr2:uid="{67120B50-DA24-409C-9D35-548584692329}"/>
   </bookViews>
@@ -50,9 +50,6 @@
     <t>M5 Washer (.5mm to 1mm thickness)</t>
   </si>
   <si>
-    <t>390mm Gantry Setup</t>
-  </si>
-  <si>
     <t>390mm T-Slot Aluminum Extrusion</t>
   </si>
   <si>
@@ -131,9 +128,6 @@
     <t>M3x8mm</t>
   </si>
   <si>
-    <t>Custom Print Head Mount</t>
-  </si>
-  <si>
     <t>M3 Brass Heat  Inserts</t>
   </si>
   <si>
@@ -164,9 +158,6 @@
     <t>M3x12mm</t>
   </si>
   <si>
-    <t>340mm Gantry Setup</t>
-  </si>
-  <si>
     <t>340mm T-Slot Aluminum Extrusion</t>
   </si>
   <si>
@@ -186,6 +177,15 @@
   </si>
   <si>
     <t>M3x30mm Socket Head</t>
+  </si>
+  <si>
+    <t>390mm Gantry Setup (Use MGN12H for  AfterBurner)</t>
+  </si>
+  <si>
+    <t>Custom Print Head Mount (Not Required if Using AfterBurner)</t>
+  </si>
+  <si>
+    <t>340mm Gantry Setup (Use MGN12H for  AfterBurner)</t>
   </si>
 </sst>
 </file>
@@ -261,13 +261,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -588,7 +588,7 @@
   <dimension ref="A1:E64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -604,22 +604,22 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>5</v>
+        <v>48</v>
       </c>
       <c r="B5" s="5"/>
       <c r="C5" s="5"/>
       <c r="D5" s="4" t="s">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="E5" s="5"/>
     </row>
@@ -640,14 +640,14 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="5">
         <v>1</v>
       </c>
       <c r="C7" s="5"/>
       <c r="D7" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="E7" s="5">
         <v>1</v>
@@ -655,14 +655,14 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B8" s="5">
         <v>1</v>
       </c>
       <c r="C8" s="5"/>
       <c r="D8" s="5" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="E8" s="5">
         <v>1</v>
@@ -670,74 +670,74 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="5">
         <v>12</v>
       </c>
       <c r="C9" s="5"/>
       <c r="D9" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E9" s="5">
         <v>6</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="B10" s="9">
+      <c r="A10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="7">
         <v>12</v>
       </c>
       <c r="C10" s="5"/>
-      <c r="D10" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="9">
+      <c r="D10" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="7">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="B11" s="9">
+      <c r="A11" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B11" s="7">
         <v>4</v>
       </c>
       <c r="C11" s="5"/>
-      <c r="D11" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="E11" s="9">
+      <c r="D11" s="7" t="s">
+        <v>46</v>
+      </c>
+      <c r="E11" s="7">
         <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B12" s="9">
+      <c r="A12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="7">
         <v>4</v>
       </c>
       <c r="C12" s="5"/>
-      <c r="D12" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E12" s="9">
+      <c r="D12" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E12" s="7">
         <v>4</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B13" s="6">
         <v>8</v>
       </c>
       <c r="C13" s="6"/>
       <c r="D13" s="6" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="E13" s="6">
         <v>8</v>
@@ -745,7 +745,7 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="B15" s="5"/>
       <c r="C15" s="5"/>
@@ -754,7 +754,7 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B16" s="5">
         <v>12</v>
@@ -765,7 +765,7 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B17" s="5">
         <v>2</v>
@@ -776,7 +776,7 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B18" s="5">
         <v>4</v>
@@ -787,7 +787,7 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B19" s="5">
         <v>3</v>
@@ -798,7 +798,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B20" s="5">
         <v>2</v>
@@ -809,7 +809,7 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B21" s="6">
         <v>1</v>
@@ -831,14 +831,14 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B24" s="5">
         <v>4</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="5" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="E24" s="5">
         <v>4</v>
@@ -861,14 +861,14 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B26" s="5">
         <v>4</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E26" s="5">
         <v>4</v>
@@ -876,14 +876,14 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B27" s="5">
         <v>4</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E27" s="5">
         <v>4</v>
@@ -891,14 +891,14 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B28" s="6">
         <v>2</v>
       </c>
       <c r="C28" s="6"/>
       <c r="D28" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E28" s="6">
         <v>2</v>
@@ -906,40 +906,40 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B30" s="5"/>
       <c r="C30" s="5"/>
-      <c r="D30" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E30" s="7"/>
+      <c r="D30" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30" s="8"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B31" s="5">
         <v>4</v>
       </c>
       <c r="C31" s="5"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B32" s="6">
         <v>4</v>
       </c>
       <c r="C32" s="6"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B34" s="5"/>
       <c r="C34" s="5"/>
@@ -948,7 +948,7 @@
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B35" s="5">
         <v>4</v>
@@ -959,7 +959,7 @@
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B36" s="5">
         <v>4</v>
@@ -970,7 +970,7 @@
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B37" s="5">
         <v>2</v>
@@ -981,7 +981,7 @@
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B38" s="6">
         <v>2</v>
@@ -992,7 +992,7 @@
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B40" s="5"/>
       <c r="C40" s="5"/>
@@ -1001,7 +1001,7 @@
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B41" s="5">
         <v>2</v>
@@ -1012,7 +1012,7 @@
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B42" s="5">
         <v>12</v>
@@ -1023,7 +1023,7 @@
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B43" s="5">
         <v>12</v>
@@ -1034,7 +1034,7 @@
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B44" s="5">
         <v>3</v>
@@ -1045,7 +1045,7 @@
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B45" s="6">
         <v>3</v>
@@ -1056,7 +1056,7 @@
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B47" s="5"/>
       <c r="C47" s="5"/>
@@ -1065,7 +1065,7 @@
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B48" s="5">
         <v>1</v>
@@ -1076,7 +1076,7 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B49" s="5">
         <v>1</v>
@@ -1087,7 +1087,7 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B50" s="5">
         <v>2</v>
@@ -1098,7 +1098,7 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B51" s="5">
         <v>2</v>
@@ -1109,7 +1109,7 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B52" s="6">
         <v>2</v>
@@ -1120,12 +1120,12 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B55">
         <v>3</v>
@@ -1133,7 +1133,7 @@
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B56">
         <v>3</v>
@@ -1141,7 +1141,7 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B57">
         <v>2</v>
@@ -1149,7 +1149,7 @@
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B58">
         <v>4</v>
@@ -1157,12 +1157,12 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B61">
         <v>2</v>
@@ -1170,7 +1170,7 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B62">
         <v>4</v>
@@ -1178,7 +1178,7 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B63">
         <v>4</v>
@@ -1186,7 +1186,7 @@
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B64">
         <v>2</v>

</xml_diff>